<commit_message>
reformat output; defect log.
</commit_message>
<xml_diff>
--- a/data/Test-Defects-E2E-MVP-CRUK.xlsx
+++ b/data/Test-Defects-E2E-MVP-CRUK.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E04ED2-776C-A748-B8F3-290CAE359620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0C9542-8F5A-8443-AB00-D550D8720F3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2420" yWindow="-20540" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="Picklists" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recording Sheet'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recording Sheet'!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -50,18 +50,9 @@
     </r>
   </si>
   <si>
-    <t>Test Step Number</t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
     <t>Test Step Header</t>
   </si>
   <si>
-    <t>Test Step Detail</t>
-  </si>
-  <si>
     <t>Defect Description</t>
   </si>
   <si>
@@ -114,6 +105,42 @@
   </si>
   <si>
     <t>Verified</t>
+  </si>
+  <si>
+    <t>Testing concordance of v1 and v2 output</t>
+  </si>
+  <si>
+    <t>Transformation of data from FTP S3 bucket to REL input bucket</t>
+  </si>
+  <si>
+    <t>Original multi-SLX data not copied from 'ftps-core-ftps3bucket-1b6k14wlq0yu7' to 'transformed-data-bucket-rel' (e.g.  'SLX-100.s_1.SRR8983578.fastq.gz'). Possibly because the filenames are not as expected - need clarification.</t>
+  </si>
+  <si>
+    <t>ATK</t>
+  </si>
+  <si>
+    <t>The order of the columns (sample names) in the 'combined_counts.txt' file seems to depend on the order of samples in the original json analysis config file even though the data is identical.</t>
+  </si>
+  <si>
+    <t>The 'neg.rank' and 'pos.rank' columns are not identical in the Mageck output - there seems to be some randomness in the ranking of tied genes. This also impacts the order of the genes in the output file.</t>
+  </si>
+  <si>
+    <t>"GeneConnectivity" interpretation output is private to AZ</t>
+  </si>
+  <si>
+    <t>"PathwayAnalysis" interpretation output is provate to v2.</t>
+  </si>
+  <si>
+    <t>"fastq" and "fastqc" sub-folders no longer saved in v2 'crisprn' sub-folder, but at the same level as 'crisprn' folder.</t>
+  </si>
+  <si>
+    <t>"counts' sub-folder within "crisprn" folder now contains the merging counts log, for v1 it contained the log for individual sample counts as well as the merging counts log.</t>
+  </si>
+  <si>
+    <t>UAT_analysis.Rmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The order of the sgRNAs in the 'combined_counts.txt' file also seems to depend on the order of the samples in the original json file (perhaps ordering of rows occurs across sample column order). </t>
   </si>
 </sst>
 </file>
@@ -178,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -194,6 +221,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,33 +566,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.1640625" style="1"/>
     <col min="2" max="2" width="16.6640625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="12.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="29.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="34.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="72.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" style="1" customWidth="1"/>
-    <col min="13" max="14" width="43.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="12.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="72.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="43.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -569,10 +602,10 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -596,18 +629,217 @@
       <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="6">
+        <v>43872</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="6">
+        <v>43872</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>14</v>
+    </row>
+    <row r="4" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="6">
+        <v>43872</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="6">
+        <v>43872</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="6">
+        <v>43872</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="6">
+        <v>43872</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="6">
+        <v>43872</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="6">
+        <v>43872</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1" xr:uid="{24E13A05-B679-4210-90AA-1EA6CC69A9C8}"/>
+  <autoFilter ref="A1:L1" xr:uid="{24E13A05-B679-4210-90AA-1EA6CC69A9C8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -617,13 +849,13 @@
           <x14:formula1>
             <xm:f>Picklists!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K20</xm:sqref>
+          <xm:sqref>H2:H20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{988B4C65-F4BB-4D29-9C1E-759B6EB14CEF}">
           <x14:formula1>
             <xm:f>Picklists!$C$1:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L20</xm:sqref>
+          <xm:sqref>I2:I20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -643,44 +875,44 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
approach section; README update.
</commit_message>
<xml_diff>
--- a/data/Test-Defects-E2E-MVP-CRUK.xlsx
+++ b/data/Test-Defects-E2E-MVP-CRUK.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0C9542-8F5A-8443-AB00-D550D8720F3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F571D3-6B49-DE46-86FF-87B2613B48AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2420" yWindow="-20540" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -137,17 +137,41 @@
     <t>"counts' sub-folder within "crisprn" folder now contains the merging counts log, for v1 it contained the log for individual sample counts as well as the merging counts log.</t>
   </si>
   <si>
-    <t>UAT_analysis.Rmd</t>
-  </si>
-  <si>
     <t xml:space="preserve">The order of the sgRNAs in the 'combined_counts.txt' file also seems to depend on the order of the samples in the original json file (perhaps ordering of rows occurs across sample column order). </t>
+  </si>
+  <si>
+    <t>https://github.com/alex-kalinka-cruk/fgc_crispr_pipeline_UAT/blob/master/analysis/UAT-analysis.Rmd</t>
+  </si>
+  <si>
+    <t>Manual test of data transformation for multi-SLX use case.</t>
+  </si>
+  <si>
+    <t># Concordance of pipeline outputs with v1</t>
+  </si>
+  <si>
+    <t># Concordance of pipeline outputs with v2</t>
+  </si>
+  <si>
+    <t># Concordance of pipeline outputs with v3</t>
+  </si>
+  <si>
+    <t># Concordance of pipeline outputs with v4</t>
+  </si>
+  <si>
+    <t># Concordance of pipeline outputs with v5</t>
+  </si>
+  <si>
+    <t># Concordance of pipeline outputs with v6</t>
+  </si>
+  <si>
+    <t># Concordance of pipeline outputs with v7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +183,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,10 +240,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -228,8 +267,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -572,7 +613,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -634,11 +675,14 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
+      <c r="B2" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
@@ -660,11 +704,14 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
+      <c r="B3" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>26</v>
@@ -686,14 +733,17 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
+      <c r="B4" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="6">
         <v>43872</v>
@@ -712,11 +762,14 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
+      <c r="B5" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>27</v>
@@ -738,11 +791,14 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
+      <c r="B6" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>28</v>
@@ -764,11 +820,14 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>32</v>
+      <c r="B7" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>29</v>
@@ -790,11 +849,14 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>32</v>
+      <c r="B8" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>30</v>
@@ -816,12 +878,15 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
+      <c r="B9" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
@@ -840,8 +905,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L1" xr:uid="{24E13A05-B679-4210-90AA-1EA6CC69A9C8}"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{AD8FC731-4B18-1644-9333-1D45E2E5ECFB}"/>
+    <hyperlink ref="B3:B9" r:id="rId2" display="https://github.com/alex-kalinka-cruk/fgc_crispr_pipeline_UAT/blob/master/analysis/UAT-analysis.Rmd" xr:uid="{64BB4C97-762A-4342-9138-1C437153A897}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>

<commit_message>
UAT results on 2020-02-11.
</commit_message>
<xml_diff>
--- a/data/Test-Defects-E2E-MVP-CRUK.xlsx
+++ b/data/Test-Defects-E2E-MVP-CRUK.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F571D3-6B49-DE46-86FF-87B2613B48AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7CA230-04BB-4948-A9A3-EBA0E1741E03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2420" yWindow="-20540" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,9 +128,6 @@
     <t>"GeneConnectivity" interpretation output is private to AZ</t>
   </si>
   <si>
-    <t>"PathwayAnalysis" interpretation output is provate to v2.</t>
-  </si>
-  <si>
     <t>"fastq" and "fastqc" sub-folders no longer saved in v2 'crisprn' sub-folder, but at the same level as 'crisprn' folder.</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t># Concordance of pipeline outputs with v7</t>
+  </si>
+  <si>
+    <t>"PathwayAnalysis" interpretation output is private to v2.</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -676,13 +676,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
@@ -705,13 +705,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>26</v>
@@ -734,16 +734,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="6">
         <v>43872</v>
@@ -763,13 +763,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>27</v>
@@ -792,13 +792,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>28</v>
@@ -821,16 +821,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F7" s="6">
         <v>43872</v>
@@ -850,16 +850,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="6">
         <v>43872</v>
@@ -879,16 +879,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="6">
         <v>43872</v>

</xml_diff>